<commit_message>
Minor corrections to pinkbike templates
</commit_message>
<xml_diff>
--- a/ExcelTemplates/FutureShopTemplate.xlsx
+++ b/ExcelTemplates/FutureShopTemplate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16380"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="16380"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -491,8 +491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>

</xml_diff>